<commit_message>
update to ontwikkel xsd-schema and oefen xsd-schema
</commit_message>
<xml_diff>
--- a/templates/oefen/oefen_bodem_template.xlsx
+++ b/templates/oefen/oefen_bodem_template.xlsx
@@ -6082,13 +6082,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-03-05 16:14:53.233749</t>
+    <t>2025-03-19 12:18:13.285115</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.1.2</t>
+    <t>2.1.3</t>
   </si>
   <si>
     <t>xdov-version</t>

</xml_diff>

<commit_message>
update to ontwikkel xsd-schema and productie xsd-schema
</commit_message>
<xml_diff>
--- a/templates/oefen/oefen_bodem_template.xlsx
+++ b/templates/oefen/oefen_bodem_template.xlsx
@@ -6082,25 +6082,25 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-03-19 12:18:13.285115</t>
+    <t>2025-04-17 10:01:24.939855</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.1.3</t>
+    <t>2.1.4</t>
   </si>
   <si>
     <t>xdov-version</t>
   </si>
   <si>
-    <t>9.1.0</t>
+    <t>9.1.2</t>
   </si>
   <si>
     <t>schema-version</t>
   </si>
   <si>
-    <t>5.4.0</t>
+    <t>5.4.1</t>
   </si>
   <si>
     <t>mode</t>

</xml_diff>

<commit_message>
fixed DOVXLS2XML-137 by adding boolean support to the templates
</commit_message>
<xml_diff>
--- a/templates/oefen/oefen_bodem_template.xlsx
+++ b/templates/oefen/oefen_bodem_template.xlsx
@@ -6085,13 +6085,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-06-27 02:17:33.814426</t>
+    <t>2025-08-06 15:10:54.407385</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.1.5</t>
+    <t>2.1.6</t>
   </si>
   <si>
     <t>xdov-version</t>
@@ -46908,7 +46908,7 @@
     <mergeCell ref="AA3:AB3"/>
     <mergeCell ref="K2:AB2"/>
   </mergeCells>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B1000001">
       <formula1>'Codelijsten'!$BK$4:$BK$6</formula1>
     </dataValidation>
@@ -46923,6 +46923,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8:M1000001">
       <formula1>'Codelijsten'!$BQ$4:$BQ$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R8:R1000001">
+      <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U1000001">
       <formula1>'Codelijsten'!$BS$4:$BS$9</formula1>

</xml_diff>

<commit_message>
update to ontwikkel and productie schema
</commit_message>
<xml_diff>
--- a/templates/oefen/oefen_bodem_template.xlsx
+++ b/templates/oefen/oefen_bodem_template.xlsx
@@ -6169,19 +6169,19 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-09-18 15:21:10.879280</t>
+    <t>2025-09-22 09:28:02.051028</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.1.7</t>
+    <t>2.1.8</t>
   </si>
   <si>
     <t>xdov-version</t>
   </si>
   <si>
-    <t>9.2.0</t>
+    <t>9.2.2</t>
   </si>
   <si>
     <t>schema-version</t>
@@ -45232,43 +45232,43 @@
   </mergeCells>
   <dataValidations count="17">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B1000001">
-      <formula1>'Codelijsten'!$A$4:$A$5</formula1>
+      <formula1>'Codelijsten'!$A$4:''$A$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C1000001">
-      <formula1>'Codelijsten'!$C$4:$C$21</formula1>
+      <formula1>'Codelijsten'!$C$4:''$C$21</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D1000001">
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G1000001">
-      <formula1>'Codelijsten'!$E$4:$E$17</formula1>
+      <formula1>'Codelijsten'!$E$4:''$E$17</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1000001">
-      <formula1>'Codelijsten'!$G$4:$G$6</formula1>
+      <formula1>'Codelijsten'!$G$4:''$G$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K9:K1000001">
-      <formula1>'Codelijsten'!$I$4:$I$20</formula1>
+      <formula1>'Codelijsten'!$I$4:''$I$20</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M1000001">
-      <formula1>'Codelijsten'!$K$4:$K$6</formula1>
+      <formula1>'Codelijsten'!$K$4:''$K$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P9:P1000001">
-      <formula1>'Codelijsten'!$M$4:$M$6</formula1>
+      <formula1>'Codelijsten'!$M$4:''$M$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q9:Q1000001">
-      <formula1>'Codelijsten'!$O$4:$O$17</formula1>
+      <formula1>'Codelijsten'!$O$4:''$O$17</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T9:T1000001">
-      <formula1>'Codelijsten'!$Q$4:$Q$6</formula1>
+      <formula1>'Codelijsten'!$Q$4:''$Q$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U9:U1000001">
-      <formula1>'Codelijsten'!$S$4:$S$20</formula1>
+      <formula1>'Codelijsten'!$S$4:''$S$20</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W9:W1000001">
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE9:AE1000001">
-      <formula1>'Codelijsten'!$U$4:$U$8</formula1>
+      <formula1>'Codelijsten'!$U$4:''$U$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF9:AF1000001">
       <formula1>-146096</formula1>
@@ -45280,7 +45280,7 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO9:AO1000001">
-      <formula1>'Codelijsten'!$W$4:$W$86</formula1>
+      <formula1>'Codelijsten'!$W$4:''$W$86</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -45640,7 +45640,7 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K1000001">
-      <formula1>'Codelijsten'!$Y$4:$Y$8</formula1>
+      <formula1>'Codelijsten'!$Y$4:''$Y$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O7:O1000001">
       <formula1>-146096</formula1>
@@ -45649,7 +45649,7 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7:S1000001">
-      <formula1>'Codelijsten'!$AA$4:$AA$86</formula1>
+      <formula1>'Codelijsten'!$AA$4:''$AA$86</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -46147,16 +46147,16 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1000001">
-      <formula1>'Codelijsten'!$AC$4:$AC$5</formula1>
+      <formula1>'Codelijsten'!$AC$4:''$AC$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G1000001">
-      <formula1>'Codelijsten'!$AE$4:$AE$6</formula1>
+      <formula1>'Codelijsten'!$AE$4:''$AE$6</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S8:S1000001">
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V8:V1000001">
-      <formula1>'Codelijsten'!$AG$4:$AG$8</formula1>
+      <formula1>'Codelijsten'!$AG$4:''$AG$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z8:Z1000001">
       <formula1>-146096</formula1>
@@ -46165,7 +46165,7 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD8:AD1000001">
-      <formula1>'Codelijsten'!$AI$4:$AI$86</formula1>
+      <formula1>'Codelijsten'!$AI$4:''$AI$86</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -46988,49 +46988,49 @@
   </mergeCells>
   <dataValidations count="16">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A9:A1000001">
-      <formula1>'Codelijsten'!$AK$4:$AK$1003</formula1>
+      <formula1>'Codelijsten'!$AK$4:''$AK$1003</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D1000001">
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E9:E1000001">
-      <formula1>'Codelijsten'!$AM$4:$AM$5</formula1>
+      <formula1>'Codelijsten'!$AM$4:''$AM$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1000001">
-      <formula1>'Codelijsten'!$AO$4:$AO$6</formula1>
+      <formula1>'Codelijsten'!$AO$4:''$AO$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O9:O1000001">
-      <formula1>'Codelijsten'!$AQ$4:$AQ$6</formula1>
+      <formula1>'Codelijsten'!$AQ$4:''$AQ$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q9:Q1000001">
-      <formula1>'Codelijsten'!$AS$4:$AS$68</formula1>
+      <formula1>'Codelijsten'!$AS$4:''$AS$68</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S9:S1000001">
-      <formula1>'Codelijsten'!$AU$4:$AU$6</formula1>
+      <formula1>'Codelijsten'!$AU$4:''$AU$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X9:X1000001">
-      <formula1>'Codelijsten'!$AW$4:$AW$181</formula1>
+      <formula1>'Codelijsten'!$AW$4:''$AW$181</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB9:AB1000001">
-      <formula1>'Codelijsten'!$AY$4:$AY$1003</formula1>
+      <formula1>'Codelijsten'!$AY$4:''$AY$1003</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE9:AE1000001">
-      <formula1>'Codelijsten'!$BA$4:$BA$68</formula1>
+      <formula1>'Codelijsten'!$BA$4:''$BA$68</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS9:AS1000001">
-      <formula1>'Codelijsten'!$BC$4:$BC$68</formula1>
+      <formula1>'Codelijsten'!$BC$4:''$BC$68</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT9:AT1000001">
-      <formula1>'Codelijsten'!$BE$4:$BE$68</formula1>
+      <formula1>'Codelijsten'!$BE$4:''$BE$68</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV9:AV1000001">
-      <formula1>'Codelijsten'!$BG$4:$BG$8</formula1>
+      <formula1>'Codelijsten'!$BG$4:''$BG$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW9:AW1000001">
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AX9:AX1000001">
-      <formula1>'Codelijsten'!$BI$4:$BI$6</formula1>
+      <formula1>'Codelijsten'!$BI$4:''$BI$6</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF9:BF1000001">
       <formula1>-146096</formula1>
@@ -47442,28 +47442,28 @@
   </mergeCells>
   <dataValidations count="9">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B8:B1000001">
-      <formula1>'Codelijsten'!$BK$4:$BK$6</formula1>
+      <formula1>'Codelijsten'!$BK$4:''$BK$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C1000001">
-      <formula1>'Codelijsten'!$BM$4:$BM$6</formula1>
+      <formula1>'Codelijsten'!$BM$4:''$BM$6</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H1000001">
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K8:K1000001">
-      <formula1>'Codelijsten'!$BO$4:$BO$5</formula1>
+      <formula1>'Codelijsten'!$BO$4:''$BO$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M8:M1000001">
-      <formula1>'Codelijsten'!$BQ$4:$BQ$6</formula1>
+      <formula1>'Codelijsten'!$BQ$4:''$BQ$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R8:R1000001">
       <formula1>"true,false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U1000001">
-      <formula1>'Codelijsten'!$BS$4:$BS$9</formula1>
+      <formula1>'Codelijsten'!$BS$4:''$BS$9</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V8:V1000001">
-      <formula1>'Codelijsten'!$BU$4:$BU$7</formula1>
+      <formula1>'Codelijsten'!$BU$4:''$BU$7</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X8:X1000001">
       <formula1>-146096</formula1>
@@ -47748,10 +47748,10 @@
   </mergeCells>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E1000001">
-      <formula1>'Codelijsten'!$BW$4:$BW$29</formula1>
+      <formula1>'Codelijsten'!$BW$4:''$BW$29</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F1000001">
-      <formula1>'Codelijsten'!$BY$4:$BY$18</formula1>
+      <formula1>'Codelijsten'!$BY$4:''$BY$18</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G1000001">
       <formula1>-146096</formula1>
@@ -47760,13 +47760,13 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6:L1000001">
-      <formula1>'Codelijsten'!$CA$4:$CA$8</formula1>
+      <formula1>'Codelijsten'!$CA$4:''$CA$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6:N1000001">
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P1000001">
-      <formula1>'Codelijsten'!$CC$4:$CC$86</formula1>
+      <formula1>'Codelijsten'!$CC$4:''$CC$86</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -48583,25 +48583,25 @@
   </mergeCells>
   <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B1000001">
-      <formula1>'Codelijsten'!$CE$4:$CE$14</formula1>
+      <formula1>'Codelijsten'!$CE$4:''$CE$14</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:C1000001">
-      <formula1>'Codelijsten'!$CG$4:$CG$5</formula1>
+      <formula1>'Codelijsten'!$CG$4:''$CG$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H1000001">
-      <formula1>'Codelijsten'!$CI$4:$CI$86</formula1>
+      <formula1>'Codelijsten'!$CI$4:''$CI$86</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I7:I1000001">
-      <formula1>'Codelijsten'!$CK$4:$CK$12</formula1>
+      <formula1>'Codelijsten'!$CK$4:''$CK$12</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T7:T1000001">
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W7:W1000001">
-      <formula1>'Codelijsten'!$CM$4:$CM$40</formula1>
+      <formula1>'Codelijsten'!$CM$4:''$CM$40</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X7:X1000001">
-      <formula1>'Codelijsten'!$CO$4:$CO$6</formula1>
+      <formula1>'Codelijsten'!$CO$4:''$CO$6</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7:AG1000001">
       <formula1>-146096</formula1>
@@ -48619,7 +48619,7 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD7:BD1000001">
-      <formula1>'Codelijsten'!$CQ$4:$CQ$86</formula1>
+      <formula1>'Codelijsten'!$CQ$4:''$CQ$86</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -49605,22 +49605,22 @@
   </mergeCells>
   <dataValidations count="15">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A8:A1000001">
-      <formula1>'Codelijsten'!$CS$4:$CS$1003</formula1>
+      <formula1>'Codelijsten'!$CS$4:''$CS$1003</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N8:N1000001">
-      <formula1>'Codelijsten'!$CU$4:$CU$68</formula1>
+      <formula1>'Codelijsten'!$CU$4:''$CU$68</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O8:O1000001">
-      <formula1>'Codelijsten'!$CW$4:$CW$68</formula1>
+      <formula1>'Codelijsten'!$CW$4:''$CW$68</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB8:AB1000001">
-      <formula1>'Codelijsten'!$CY$4:$CY$68</formula1>
+      <formula1>'Codelijsten'!$CY$4:''$CY$68</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC8:AC1000001">
-      <formula1>'Codelijsten'!$DA$4:$DA$6</formula1>
+      <formula1>'Codelijsten'!$DA$4:''$DA$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD8:AD1000001">
-      <formula1>'Codelijsten'!$DC$4:$DC$181</formula1>
+      <formula1>'Codelijsten'!$DC$4:''$DC$181</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE8:AE1000001">
       <formula1>-146096</formula1>
@@ -49629,13 +49629,13 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG8:AG1000001">
-      <formula1>'Codelijsten'!$DE$4:$DE$6</formula1>
+      <formula1>'Codelijsten'!$DE$4:''$DE$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY8:AY1000001">
-      <formula1>'Codelijsten'!$DG$4:$DG$1003</formula1>
+      <formula1>'Codelijsten'!$DG$4:''$DG$1003</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB8:BB1000001">
-      <formula1>'Codelijsten'!$DI$4:$DI$68</formula1>
+      <formula1>'Codelijsten'!$DI$4:''$DI$68</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BE8:BE1000001">
       <formula1>-146096</formula1>
@@ -49647,7 +49647,7 @@
       <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR8:BR1000001">
-      <formula1>'Codelijsten'!$DK$4:$DK$86</formula1>
+      <formula1>'Codelijsten'!$DK$4:''$DK$86</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>

<commit_message>
Updates to xls2xml.exe and better error-handling in validation.py
</commit_message>
<xml_diff>
--- a/templates/oefen/oefen_bodem_template.xlsx
+++ b/templates/oefen/oefen_bodem_template.xlsx
@@ -6169,13 +6169,13 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2025-09-22 11:00:04.857771</t>
+    <t>2025-09-24 17:44:35.023536</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.1.8</t>
+    <t>2.2.0</t>
   </si>
   <si>
     <t>xdov-version</t>

</xml_diff>

<commit_message>
update to xsd schemas
</commit_message>
<xml_diff>
--- a/templates/oefen/oefen_bodem_template.xlsx
+++ b/templates/oefen/oefen_bodem_template.xlsx
@@ -6127,25 +6127,25 @@
     <t>Date generated</t>
   </si>
   <si>
-    <t>2026-01-01 02:16:40.961352</t>
+    <t>2026-02-10 16:32:13.449275</t>
   </si>
   <si>
     <t>version</t>
   </si>
   <si>
-    <t>2.2.2</t>
+    <t>2.2.3</t>
   </si>
   <si>
     <t>xdov-version</t>
   </si>
   <si>
-    <t>9.4.0</t>
+    <t>9.4.3</t>
   </si>
   <si>
     <t>schema-version</t>
   </si>
   <si>
-    <t>5.7.0</t>
+    <t>5.9.0</t>
   </si>
   <si>
     <t>mode</t>

</xml_diff>